<commit_message>
chore: Updating executions and output sheets.
</commit_message>
<xml_diff>
--- a/data/processed/df_importance.xlsx
+++ b/data/processed/df_importance.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJETOS NO GIT\01 - Carne de Pescoço\ethereum_laundering\data\processed\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A2D170-C5B9-4698-A977-EE53A32343AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -139,8 +133,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,21 +197,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -255,7 +241,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -289,7 +275,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -324,10 +309,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -500,21 +484,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -522,7 +499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -530,10 +507,10 @@
         <v>22</v>
       </c>
       <c r="C2">
-        <v>9.8255607085309862</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9.825560708530986</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -541,10 +518,10 @@
         <v>63</v>
       </c>
       <c r="C3">
-        <v>406.62451362557482</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>406.6245136255748</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -555,7 +532,7 @@
         <v>3888.873594045363</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -563,10 +540,10 @@
         <v>31</v>
       </c>
       <c r="C5">
-        <v>60.380289722136688</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>60.38028972213669</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -574,10 +551,10 @@
         <v>26</v>
       </c>
       <c r="C6">
-        <v>181.71878996315351</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>181.7187899631535</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -585,10 +562,10 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>8.7714522182941437</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8.771452218294144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -596,10 +573,10 @@
         <v>160</v>
       </c>
       <c r="C8">
-        <v>830.03624021523228</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>830.0362402152323</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -607,10 +584,10 @@
         <v>25</v>
       </c>
       <c r="C9">
-        <v>7.5149674545064036</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7.514967454506404</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -618,10 +595,10 @@
         <v>25</v>
       </c>
       <c r="C10">
-        <v>47.648869268596172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>47.64886926859617</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -629,10 +606,10 @@
         <v>33</v>
       </c>
       <c r="C11">
-        <v>101.10505566733789</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>101.1050556673379</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -640,10 +617,10 @@
         <v>82</v>
       </c>
       <c r="C12">
-        <v>656.29551499157617</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>656.2955149915762</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -651,10 +628,10 @@
         <v>50</v>
       </c>
       <c r="C13">
-        <v>200.25604570625731</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>200.2560457062573</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -665,7 +642,7 @@
         <v>10.7715220451355</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -673,10 +650,10 @@
         <v>23</v>
       </c>
       <c r="C15">
-        <v>64.533722168882377</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>64.53372216888238</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -687,7 +664,7 @@
         <v>1241.52320741117</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -698,7 +675,7 @@
         <v>15.03722193650901</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -706,10 +683,10 @@
         <v>33</v>
       </c>
       <c r="C18">
-        <v>453.91012918018708</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>453.9101291801871</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -717,10 +694,10 @@
         <v>65</v>
       </c>
       <c r="C19">
-        <v>759.32909501437098</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>759.329095014371</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -728,10 +705,10 @@
         <v>109</v>
       </c>
       <c r="C20">
-        <v>2432.3685398956509</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2432.368539895651</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -739,10 +716,10 @@
         <v>53</v>
       </c>
       <c r="C21">
-        <v>352.42950563955952</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>352.4295056395595</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -750,10 +727,10 @@
         <v>10</v>
       </c>
       <c r="C22">
-        <v>7.5363933009502944</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7.536393300950294</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -764,7 +741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -772,10 +749,10 @@
         <v>19</v>
       </c>
       <c r="C24">
-        <v>40.814324602484703</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40.8143246024847</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -783,10 +760,10 @@
         <v>15</v>
       </c>
       <c r="C25">
-        <v>20.579686932265759</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20.57968693226576</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -794,10 +771,10 @@
         <v>34</v>
       </c>
       <c r="C26">
-        <v>70.481048094225116</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>70.48104809422512</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
@@ -808,7 +785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -816,10 +793,10 @@
         <v>61</v>
       </c>
       <c r="C28">
-        <v>189.23404010385269</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>189.2340401038527</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
@@ -830,7 +807,7 @@
         <v>10283.85591027141</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -838,10 +815,10 @@
         <v>24</v>
       </c>
       <c r="C30">
-        <v>48.266334716542588</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>48.26633471654259</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
@@ -849,10 +826,10 @@
         <v>32</v>
       </c>
       <c r="C31">
-        <v>140.51849013566971</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>140.5184901356697</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
@@ -860,10 +837,10 @@
         <v>8</v>
       </c>
       <c r="C32">
-        <v>11.072166204452509</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11.07216620445251</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -874,7 +851,7 @@
         <v>11.53012016415596</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
@@ -882,10 +859,10 @@
         <v>25</v>
       </c>
       <c r="C34">
-        <v>43.488101355731487</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43.48810135573149</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
@@ -893,10 +870,10 @@
         <v>5</v>
       </c>
       <c r="C35">
-        <v>19.834000110626221</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19.83400011062622</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
@@ -907,7 +884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
@@ -915,7 +892,7 @@
         <v>52</v>
       </c>
       <c r="C37">
-        <v>588.23096197843552</v>
+        <v>588.2309619784355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>